<commit_message>
final: Add compiler optimisation section
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/doc/gantt/prco_time_plan.xlsx
+++ b/doc/gantt/prco_time_plan.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\uni\prco304\doc\gantt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\XilinxVM\prco304\doc\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85193C7-6B83-4071-A982-44D9F3B815A6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{F166F07A-0375-4A16-B899-B830BBC88168}"/>
   </bookViews>
@@ -1907,11 +1908,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.49981</cdr:x>
+      <cdr:x>0.70489</cdr:x>
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.50987</cdr:x>
+      <cdr:x>0.71495</cdr:x>
       <cdr:y>1</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -1927,8 +1928,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="5060585" y="0"/>
-          <a:ext cx="101858" cy="6086475"/>
+          <a:off x="7137064" y="0"/>
+          <a:ext cx="101859" cy="6086475"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2419,7 +2420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81979E81-6286-4617-9260-EEEC38151FA0}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
final: Add kanban board and explain emulator output
Signed-off-by: Ben Lancaster <bdl@live.co.uk>
</commit_message>
<xml_diff>
--- a/doc/gantt/prco_time_plan.xlsx
+++ b/doc/gantt/prco_time_plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\XilinxVM\prco304\doc\gantt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85193C7-6B83-4071-A982-44D9F3B815A6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BC331B-7B87-46B9-A4A4-6D4746A9B7E3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" xr2:uid="{F166F07A-0375-4A16-B899-B830BBC88168}"/>
   </bookViews>
@@ -1908,11 +1908,11 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.70489</cdr:x>
+      <cdr:x>0.55719</cdr:x>
       <cdr:y>0</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.71495</cdr:x>
+      <cdr:x>0.56725</cdr:x>
       <cdr:y>1</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
@@ -1928,8 +1928,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="7137064" y="0"/>
-          <a:ext cx="101859" cy="6086475"/>
+          <a:off x="5641640" y="0"/>
+          <a:ext cx="101858" cy="6086475"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2420,8 +2420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81979E81-6286-4617-9260-EEEC38151FA0}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>